<commit_message>
fix multiple quantity item not showing multi row
</commit_message>
<xml_diff>
--- a/tests/bigseller/data.input/bigseller.input.order.sample.xlsx
+++ b/tests/bigseller/data.input/bigseller.input.order.sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\cardeco\tests\bigseller\data.input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BB1C43-7968-4BB5-8065-3CDDFF48679F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020B2B29-36B3-4C61-82C0-29F3D8F03485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3AD1A54-25DF-4154-82AF-536F017A445B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="272">
   <si>
     <t>Order No</t>
   </si>
@@ -859,6 +859,9 @@
   </si>
   <si>
     <t>456, Kampung Y, IN</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -1236,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984D95CF-2B9B-4C40-9A78-EF3A3A473489}">
   <dimension ref="A1:BN11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI5" sqref="AI5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,7 +2352,7 @@
         <v>167</v>
       </c>
       <c r="AI6" s="2" t="s">
-        <v>89</v>
+        <v>271</v>
       </c>
       <c r="AJ6" s="2" t="s">
         <v>167</v>

</xml_diff>

<commit_message>
change marketplace to store name, update tests data
</commit_message>
<xml_diff>
--- a/tests/bigseller/data.input/bigseller.input.order.sample.xlsx
+++ b/tests/bigseller/data.input/bigseller.input.order.sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\cardeco\tests\bigseller\data.input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF83AB0-4D81-462B-9ACF-AC03DD65872E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F43DF0A-3257-4D7C-B2EA-C47825A80595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3AD1A54-25DF-4154-82AF-536F017A445B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="313">
   <si>
     <t>Order No</t>
   </si>
@@ -318,9 +318,6 @@
   </si>
   <si>
     <t>M******n</t>
-  </si>
-  <si>
-    <t>******91</t>
   </si>
   <si>
     <t>Tebrau</t>
@@ -623,9 +620,6 @@
     <t>44.1</t>
   </si>
   <si>
-    <t>2023-07-07 18:50</t>
-  </si>
-  <si>
     <t>2023-07-07 18:51</t>
   </si>
   <si>
@@ -648,37 +642,6 @@
   </si>
   <si>
     <t>8.55</t>
-  </si>
-  <si>
-    <t>577544991388764355</t>
-  </si>
-  <si>
-    <t>BS69KX074698</t>
-  </si>
-  <si>
-    <t>M*** A*** B** A***</t>
-  </si>
-  <si>
-    <t>17***</t>
-  </si>
-  <si>
-    <t>Car Door Window Pillar Trim Cover (Black / Chrome / Gold / Rose) - HONDA Accord, City, Civic, Hrv, Jazz</t>
-  </si>
-  <si>
-    <t>EX-1001-ACC03</t>
-  </si>
-  <si>
-    <t>Accord 2003-2007 (4pcs), Chrome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://p16-oec-va.ibyteimg.com/tos-maliva-i-o3syd03w52-us/b8afbe1d888f4f079c91a3059655699d~tplv-o3syd03w52-origin-jpeg.jpeg?from=1413970683_x000D_
-</t>
-  </si>
-  <si>
-    <t>685823528310</t>
-  </si>
-  <si>
-    <t>59.9</t>
   </si>
   <si>
     <t>16800</t>
@@ -994,9 +957,6 @@
     <t>***user5</t>
   </si>
   <si>
-    <t>***user6</t>
-  </si>
-  <si>
     <t>***user7</t>
   </si>
   <si>
@@ -1022,6 +982,12 @@
   </si>
   <si>
     <t>p* ***</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>fake not founds from diff platform</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1035,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1087,6 +1053,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1101,7 +1079,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1114,6 +1092,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1429,10 +1415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984D95CF-2B9B-4C40-9A78-EF3A3A473489}">
-  <dimension ref="A1:BO15"/>
+  <dimension ref="A1:BO17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AC15" sqref="AC15"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,7 +1534,7 @@
         <v>34</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>35</v>
@@ -1646,10 +1632,10 @@
     </row>
     <row r="2" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>66</v>
@@ -1658,10 +1644,10 @@
         <v>67</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>85</v>
@@ -1676,76 +1662,76 @@
         <v>66</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="Z2" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AB2" s="2" t="s">
         <v>73</v>
       </c>
       <c r="AC2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD2" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG2" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AF2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="AI2" s="2" t="s">
         <v>74</v>
@@ -1754,7 +1740,7 @@
         <v>67</v>
       </c>
       <c r="AK2" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AL2" s="2" t="s">
         <v>67</v>
@@ -1769,10 +1755,10 @@
         <v>67</v>
       </c>
       <c r="AP2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="AR2" s="2" t="s">
         <v>67</v>
@@ -1787,10 +1773,10 @@
         <v>79</v>
       </c>
       <c r="AV2" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AW2" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AX2" s="2" t="s">
         <v>78</v>
@@ -1808,13 +1794,13 @@
         <v>78</v>
       </c>
       <c r="BC2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BD2" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="BE2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BF2" s="2" t="s">
         <v>92</v>
@@ -1849,10 +1835,10 @@
     </row>
     <row r="3" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>66</v>
@@ -1861,10 +1847,10 @@
         <v>67</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>69</v>
@@ -1879,76 +1865,76 @@
         <v>66</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y3" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="Z3" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AB3" s="2" t="s">
         <v>73</v>
       </c>
       <c r="AC3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AD3" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG3" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="AF3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG3" s="2" t="s">
+      <c r="AH3" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="AI3" s="2" t="s">
         <v>74</v>
@@ -1957,25 +1943,25 @@
         <v>67</v>
       </c>
       <c r="AK3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="AL3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AQ3" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="AR3" s="2" t="s">
         <v>67</v>
@@ -1990,7 +1976,7 @@
         <v>79</v>
       </c>
       <c r="AV3" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AW3" s="2" t="s">
         <v>78</v>
@@ -2008,19 +1994,19 @@
         <v>81</v>
       </c>
       <c r="BB3" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="BC3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BD3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BE3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BF3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BG3" s="2" t="s">
         <v>67</v>
@@ -2052,10 +2038,10 @@
     </row>
     <row r="4" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>66</v>
@@ -2082,100 +2068,100 @@
         <v>66</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="V4" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="W4" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="X4" s="2" t="s">
         <v>67</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AB4" s="2" t="s">
         <v>73</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AD4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE4" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="AE4" s="2" t="s">
+      <c r="AF4" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="AF4" s="2" t="s">
+      <c r="AG4" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="AH4" s="2" t="s">
         <v>91</v>
       </c>
       <c r="AI4" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AJ4" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AK4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP4" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="AL4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP4" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="AQ4" s="2" t="s">
         <v>67</v>
@@ -2190,10 +2176,10 @@
         <v>78</v>
       </c>
       <c r="AU4" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AV4" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AW4" s="2" t="s">
         <v>78</v>
@@ -2202,16 +2188,16 @@
         <v>78</v>
       </c>
       <c r="AY4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AZ4" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="AZ4" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="BA4" s="2" t="s">
         <v>81</v>
       </c>
       <c r="BB4" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BC4" s="2" t="s">
         <v>67</v>
@@ -2255,10 +2241,10 @@
     </row>
     <row r="5" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>66</v>
@@ -2267,10 +2253,10 @@
         <v>67</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>69</v>
@@ -2285,17 +2271,17 @@
         <v>66</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="O5" s="2" t="s">
         <v>67</v>
       </c>
@@ -2312,16 +2298,16 @@
         <v>67</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="X5" s="2" t="s">
         <v>67</v>
@@ -2330,31 +2316,31 @@
         <v>67</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AB5" s="2" t="s">
         <v>73</v>
       </c>
       <c r="AC5" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="AD5" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="AD5" s="2" t="s">
+      <c r="AE5" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AF5" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="AE5" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="AF5" s="2" t="s">
+      <c r="AG5" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="AG5" s="2" t="s">
+      <c r="AH5" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="AH5" s="2" t="s">
-        <v>190</v>
       </c>
       <c r="AI5" s="2" t="s">
         <v>74</v>
@@ -2363,7 +2349,7 @@
         <v>67</v>
       </c>
       <c r="AK5" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AL5" s="2" t="s">
         <v>67</v>
@@ -2381,13 +2367,13 @@
         <v>75</v>
       </c>
       <c r="AQ5" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AR5" s="2" t="s">
         <v>90</v>
       </c>
       <c r="AS5" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AT5" s="2" t="s">
         <v>78</v>
@@ -2396,10 +2382,10 @@
         <v>79</v>
       </c>
       <c r="AV5" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AW5" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AX5" s="2" t="s">
         <v>78</v>
@@ -2414,7 +2400,7 @@
         <v>81</v>
       </c>
       <c r="BB5" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BC5" s="2" t="s">
         <v>67</v>
@@ -2456,418 +2442,418 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:67" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N6" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="O6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="V6" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="W6" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="X6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y6" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z6" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="AA6" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="AB6" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC6" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD6" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE6" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AF6" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="AG6" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH6" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI6" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="AJ6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK6" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="AL6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP6" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ6" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU6" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV6" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="AW6" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="AX6" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="BB6" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="BC6" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="BD6" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="BE6" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="BF6" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="BG6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="BL6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BM6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="BN6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="BO6" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:67" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="D7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="K7" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K6" s="2" t="s">
+      <c r="L7" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="S7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="W7" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="X7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y7" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z7" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="AA7" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="AB7" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC7" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD7" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE7" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AF7" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="AG7" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH7" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI7" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK7" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="AL7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP7" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="N6" s="2" t="s">
+      <c r="AQ7" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU7" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV7" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="AW7" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="Z6" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="AA6" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="AB6" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC6" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="AE6" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="AF6" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="AG6" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="AH6" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="AI6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AK6" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="AL6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP6" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AQ6" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="AR6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AS6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AT6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AU6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AV6" s="2" t="s">
+      <c r="AX7" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA7" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="BB7" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="AW6" s="2" t="s">
+      <c r="BC7" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="BD7" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="BE7" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="BF7" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="AX6" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AY6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AZ6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BA6" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="BB6" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="BC6" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="BD6" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="BE6" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="BF6" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="BG6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BI6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BJ6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BK6" s="2" t="s">
+      <c r="BG7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK7" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="BL6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BM6" s="2" t="s">
+      <c r="BL7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BM7" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="BN6" s="2" t="s">
+      <c r="BN7" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="BO6" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z7" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC7" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="AD7" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="AE7" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="AF7" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="AG7" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="AH7" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="AI7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AK7" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="AL7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AQ7" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="AR7" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AS7" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="AT7" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AU7" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AV7" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="AW7" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AX7" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AY7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AZ7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BA7" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="BB7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="BC7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BD7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BE7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BI7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BJ7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BK7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="BL7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BM7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="BN7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="BO7" s="2" t="s">
+      <c r="BO7" s="8" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>66</v>
@@ -2897,13 +2883,13 @@
         <v>72</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>67</v>
@@ -2921,49 +2907,49 @@
         <v>67</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="X8" s="2" t="s">
         <v>67</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AA8" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AB8" s="2" t="s">
         <v>73</v>
       </c>
       <c r="AC8" s="2" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="AE8" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AF8" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AG8" s="2" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="AH8" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AI8" s="2" t="s">
         <v>74</v>
@@ -2972,7 +2958,7 @@
         <v>67</v>
       </c>
       <c r="AK8" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL8" s="2" t="s">
         <v>67</v>
@@ -3005,7 +2991,7 @@
         <v>79</v>
       </c>
       <c r="AV8" s="2" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="AW8" s="2" t="s">
         <v>80</v>
@@ -3014,10 +3000,10 @@
         <v>78</v>
       </c>
       <c r="AY8" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AZ8" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="BA8" s="2" t="s">
         <v>81</v>
@@ -3067,10 +3053,10 @@
     </row>
     <row r="9" spans="1:67" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>66</v>
@@ -3100,13 +3086,13 @@
         <v>72</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="O9" s="4" t="s">
         <v>67</v>
@@ -3124,58 +3110,58 @@
         <v>67</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="X9" s="4" t="s">
         <v>67</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AB9" s="4" t="s">
         <v>73</v>
       </c>
       <c r="AC9" s="4" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="AD9" s="4" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="AE9" s="4" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="AF9" s="4" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="AG9" s="4" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="AH9" s="4" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="AI9" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AJ9" s="4" t="s">
         <v>67</v>
       </c>
       <c r="AK9" s="4" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="AL9" s="4" t="s">
         <v>67</v>
@@ -3208,7 +3194,7 @@
         <v>79</v>
       </c>
       <c r="AV9" s="4" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="AW9" s="4" t="s">
         <v>78</v>
@@ -3217,16 +3203,16 @@
         <v>78</v>
       </c>
       <c r="AY9" s="4" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="AZ9" s="4" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="BA9" s="4" t="s">
         <v>81</v>
       </c>
       <c r="BB9" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BC9" s="4" t="s">
         <v>67</v>
@@ -3270,10 +3256,10 @@
     </row>
     <row r="10" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>66</v>
@@ -3303,13 +3289,13 @@
         <v>72</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>67</v>
@@ -3327,49 +3313,49 @@
         <v>67</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="U10" s="2" t="s">
         <v>93</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="X10" s="2" t="s">
         <v>67</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AB10" s="2" t="s">
         <v>73</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="AD10" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AE10" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="AE10" s="2" t="s">
+      <c r="AF10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG10" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="AF10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AG10" s="2" t="s">
+      <c r="AH10" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="AH10" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="AI10" s="2" t="s">
         <v>74</v>
@@ -3378,7 +3364,7 @@
         <v>67</v>
       </c>
       <c r="AK10" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AL10" s="2" t="s">
         <v>67</v>
@@ -3411,7 +3397,7 @@
         <v>79</v>
       </c>
       <c r="AV10" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AW10" s="2" t="s">
         <v>78</v>
@@ -3420,10 +3406,10 @@
         <v>78</v>
       </c>
       <c r="AY10" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AZ10" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="AZ10" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="BA10" s="2" t="s">
         <v>81</v>
@@ -3473,10 +3459,10 @@
     </row>
     <row r="11" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>66</v>
@@ -3485,10 +3471,10 @@
         <v>67</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>85</v>
@@ -3503,16 +3489,16 @@
         <v>66</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>67</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>67</v>
@@ -3530,49 +3516,49 @@
         <v>67</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="U11" s="2" t="s">
         <v>93</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="X11" s="2" t="s">
         <v>67</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="Z11" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AB11" s="2" t="s">
         <v>73</v>
       </c>
       <c r="AC11" s="2" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="AE11" s="2" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="AF11" s="2" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="AG11" s="2" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="AH11" s="2" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="AI11" s="2" t="s">
         <v>74</v>
@@ -3581,7 +3567,7 @@
         <v>67</v>
       </c>
       <c r="AK11" s="2" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="AL11" s="2" t="s">
         <v>67</v>
@@ -3596,25 +3582,25 @@
         <v>67</v>
       </c>
       <c r="AP11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ11" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="AQ11" s="2" t="s">
+      <c r="AR11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU11" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AR11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AS11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AT11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AU11" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="AV11" s="2" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="AW11" s="2" t="s">
         <v>78</v>
@@ -3635,16 +3621,16 @@
         <v>92</v>
       </c>
       <c r="BC11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BD11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BE11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BF11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BG11" s="2" t="s">
         <v>67</v>
@@ -3676,10 +3662,10 @@
     </row>
     <row r="12" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>66</v>
@@ -3688,10 +3674,10 @@
         <v>67</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>85</v>
@@ -3706,16 +3692,16 @@
         <v>66</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>67</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>67</v>
@@ -3733,49 +3719,49 @@
         <v>67</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="U12" s="2" t="s">
         <v>93</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="X12" s="2" t="s">
         <v>67</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AB12" s="2" t="s">
         <v>73</v>
       </c>
       <c r="AC12" s="2" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="AG12" s="2" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="AH12" s="2" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="AI12" s="2" t="s">
         <v>74</v>
@@ -3784,7 +3770,7 @@
         <v>67</v>
       </c>
       <c r="AK12" s="2" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="AL12" s="2" t="s">
         <v>67</v>
@@ -3799,10 +3785,10 @@
         <v>67</v>
       </c>
       <c r="AP12" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ12" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="AQ12" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="AR12" s="2" t="s">
         <v>67</v>
@@ -3817,7 +3803,7 @@
         <v>79</v>
       </c>
       <c r="AV12" s="2" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="AW12" s="2" t="s">
         <v>78</v>
@@ -3835,19 +3821,19 @@
         <v>81</v>
       </c>
       <c r="BB12" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="BC12" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BD12" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BE12" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BF12" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="BG12" s="2" t="s">
         <v>67</v>
@@ -3879,10 +3865,10 @@
     </row>
     <row r="13" spans="1:67" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>66</v>
@@ -3912,13 +3898,13 @@
         <v>72</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="O13" s="4" t="s">
         <v>67</v>
@@ -3936,58 +3922,58 @@
         <v>67</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="U13" s="2" t="s">
         <v>93</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="X13" s="4" t="s">
         <v>67</v>
       </c>
       <c r="Y13" s="4" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AB13" s="4" t="s">
         <v>73</v>
       </c>
       <c r="AC13" s="4" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="AD13" s="4" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="AE13" s="4" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="AF13" s="4" t="s">
         <v>87</v>
       </c>
       <c r="AG13" s="4" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="AH13" s="4" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="AI13" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AJ13" s="4" t="s">
         <v>67</v>
       </c>
       <c r="AK13" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AL13" s="4" t="s">
         <v>67</v>
@@ -4020,7 +4006,7 @@
         <v>79</v>
       </c>
       <c r="AV13" s="4" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="AW13" s="4" t="s">
         <v>78</v>
@@ -4029,10 +4015,10 @@
         <v>78</v>
       </c>
       <c r="AY13" s="4" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="AZ13" s="4" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="BA13" s="4" t="s">
         <v>81</v>
@@ -4082,10 +4068,10 @@
     </row>
     <row r="14" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>66</v>
@@ -4115,13 +4101,13 @@
         <v>72</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>67</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>67</v>
@@ -4139,49 +4125,49 @@
         <v>67</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="U14" s="2" t="s">
         <v>93</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="X14" s="2" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="Z14" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AA14" s="2" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="AB14" s="2" t="s">
         <v>73</v>
       </c>
       <c r="AC14" s="2" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="AD14" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE14" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AE14" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="AF14" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AG14" s="2" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="AH14" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AI14" s="2" t="s">
         <v>74</v>
@@ -4190,7 +4176,7 @@
         <v>67</v>
       </c>
       <c r="AK14" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AL14" s="2" t="s">
         <v>67</v>
@@ -4220,10 +4206,10 @@
         <v>78</v>
       </c>
       <c r="AU14" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AV14" s="2" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="AW14" s="2" t="s">
         <v>78</v>
@@ -4232,16 +4218,16 @@
         <v>78</v>
       </c>
       <c r="AY14" s="2" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="AZ14" s="2" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="BA14" s="2" t="s">
         <v>81</v>
       </c>
       <c r="BB14" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="BC14" s="2" t="s">
         <v>67</v>
@@ -4283,206 +4269,612 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="C15" s="2" t="s">
+    <row r="15" spans="1:67" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="D15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="S15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="T15" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="U15" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="V15" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="W15" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="X15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y15" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z15" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="AA15" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="AB15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC15" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD15" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE15" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="AF15" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="AG15" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH15" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI15" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="AJ15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK15" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AL15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP15" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ15" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU15" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV15" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="AW15" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="AX15" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="BB15" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="BC15" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="BD15" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="BE15" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="BF15" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="BG15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="BL15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BM15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="BN15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="BO15" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:67" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G16" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="R16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="S16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="T16" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="U16" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="V16" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="W16" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="X16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y16" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z16" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="AA16" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="AB16" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC16" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD16" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="AE16" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="AF16" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="AG16" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH16" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AI16" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AJ16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK16" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AL16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP16" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ16" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="AR16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU16" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV16" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="AW16" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="AX16" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA16" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="BB16" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="BC16" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="BD16" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="BE16" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="BF16" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="BG16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="BL16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BM16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="BN16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="BO16" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K15" s="2" t="s">
+      <c r="L17" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="X17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z17" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AA17" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AB17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC17" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="AD17" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AE17" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AF17" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="AG17" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="AH17" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="AI17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK17" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="AL17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AP17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ17" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="L15" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="V15" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="W15" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="X15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z15" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="AA15" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="AB15" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC15" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="AD15" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="AE15" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="AF15" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="AG15" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="AH15" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="AI15" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AK15" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="AL15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP15" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AQ15" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="AR15" s="2" t="s">
+      <c r="AR17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AS15" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="AT15" s="2" t="s">
+      <c r="AS17" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="AT17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AU15" s="2" t="s">
+      <c r="AU17" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AV15" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="AW15" s="2" t="s">
+      <c r="AV17" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="AW17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AX15" s="2" t="s">
+      <c r="AX17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AY15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AZ15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BA15" s="2" t="s">
+      <c r="AY17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BA17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="BB15" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="BC15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BD15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BE15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BF15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BH15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BI15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BJ15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BK15" s="2" t="s">
+      <c r="BB17" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="BC17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BE17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BF17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BI17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BJ17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BL15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BM15" s="2" t="s">
+      <c r="BL17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BM17" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="BN15" s="2" t="s">
+      <c r="BN17" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="BO15" s="2" t="s">
+      <c r="BO17" s="2" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change voucher to store voucher
</commit_message>
<xml_diff>
--- a/tests/bigseller/data.input/bigseller.input.order.sample.xlsx
+++ b/tests/bigseller/data.input/bigseller.input.order.sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\cardeco\tests\bigseller\data.input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F43DF0A-3257-4D7C-B2EA-C47825A80595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411BE3C3-45F5-4DD2-B05B-D0ADD688EF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3AD1A54-25DF-4154-82AF-536F017A445B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="315">
   <si>
     <t>Order No</t>
   </si>
@@ -988,6 +988,12 @@
   </si>
   <si>
     <t>fake not founds from diff platform</t>
+  </si>
+  <si>
+    <t>1.54</t>
+  </si>
+  <si>
+    <t>54321.23</t>
   </si>
 </sst>
 </file>
@@ -1417,8 +1423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984D95CF-2B9B-4C40-9A78-EF3A3A473489}">
   <dimension ref="A1:BO17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AE16" sqref="AE16"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AX3" sqref="AX3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1982,7 +1988,7 @@
         <v>78</v>
       </c>
       <c r="AX3" s="2" t="s">
-        <v>78</v>
+        <v>313</v>
       </c>
       <c r="AY3" s="2" t="s">
         <v>67</v>
@@ -2185,7 +2191,7 @@
         <v>78</v>
       </c>
       <c r="AX4" s="2" t="s">
-        <v>78</v>
+        <v>167</v>
       </c>
       <c r="AY4" s="2" t="s">
         <v>146</v>
@@ -2591,7 +2597,7 @@
         <v>197</v>
       </c>
       <c r="AX6" s="8" t="s">
-        <v>78</v>
+        <v>314</v>
       </c>
       <c r="AY6" s="8" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
update bigseller daily order input file format
</commit_message>
<xml_diff>
--- a/tests/bigseller/data.input/bigseller.input.order.sample.xlsx
+++ b/tests/bigseller/data.input/bigseller.input.order.sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\cardeco\tests\bigseller\data.input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411BE3C3-45F5-4DD2-B05B-D0ADD688EF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF3DAB5-270F-4624-98CC-16A2A7E16A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3AD1A54-25DF-4154-82AF-536F017A445B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="317">
   <si>
     <t>Order No</t>
   </si>
@@ -994,6 +994,12 @@
   </si>
   <si>
     <t>54321.23</t>
+  </si>
+  <si>
+    <t>Status Before Canceled</t>
+  </si>
+  <si>
+    <t>Cancellation Reason</t>
   </si>
 </sst>
 </file>
@@ -1125,9 +1131,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1165,7 +1171,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1271,7 +1277,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1413,7 +1419,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1421,19 +1427,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984D95CF-2B9B-4C40-9A78-EF3A3A473489}">
-  <dimension ref="A1:BO17"/>
+  <dimension ref="A1:BQ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AX3" sqref="AX3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="66" width="17.140625" customWidth="1"/>
+    <col min="2" max="67" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:69" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1462,181 +1468,187 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="BQ1" s="1" t="s">
+        <v>316</v>
+      </c>
     </row>
-    <row r="2" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:69" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>112</v>
       </c>
@@ -1668,14 +1680,14 @@
         <v>66</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="N2" s="2" t="s">
         <v>67</v>
       </c>
@@ -1695,62 +1707,62 @@
         <v>67</v>
       </c>
       <c r="T2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="X2" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="Y2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="AA2" s="2" t="s">
         <v>295</v>
       </c>
       <c r="AB2" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AF2" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AG2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH2" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AJ2" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AK2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL2" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AL2" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AM2" s="2" t="s">
         <v>67</v>
       </c>
@@ -1761,14 +1773,14 @@
         <v>67</v>
       </c>
       <c r="AP2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="AR2" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AS2" s="2" t="s">
         <v>67</v>
       </c>
@@ -1776,44 +1788,44 @@
         <v>67</v>
       </c>
       <c r="AU2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV2" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AV2" s="2" t="s">
+      <c r="AW2" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="AW2" s="2" t="s">
+      <c r="AX2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AX2" s="2" t="s">
+      <c r="AY2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AY2" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AZ2" s="2" t="s">
         <v>67</v>
       </c>
       <c r="BA2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="BB2" s="2" t="s">
+      <c r="BC2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="BC2" s="2" t="s">
+      <c r="BD2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="BD2" s="2" t="s">
+      <c r="BE2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="BE2" s="2" t="s">
+      <c r="BF2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="BF2" s="2" t="s">
+      <c r="BG2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="BG2" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BH2" s="2" t="s">
         <v>67</v>
       </c>
@@ -1824,22 +1836,26 @@
         <v>67</v>
       </c>
       <c r="BK2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BL2" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BM2" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN2" s="2" t="s">
         <v>84</v>
       </c>
       <c r="BO2" s="2" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ2" s="2"/>
     </row>
-    <row r="3" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:69" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>121</v>
       </c>
@@ -1871,20 +1887,20 @@
         <v>66</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="N3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="P3" s="2" t="s">
         <v>67</v>
       </c>
@@ -1898,62 +1914,62 @@
         <v>67</v>
       </c>
       <c r="T3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="X3" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="Y3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z3" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="AA3" s="2" t="s">
         <v>295</v>
       </c>
       <c r="AB3" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AE3" s="2" t="s">
+      <c r="AF3" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AF3" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AG3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH3" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="AH3" s="2" t="s">
+      <c r="AI3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AJ3" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AK3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="AL3" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AM3" s="2" t="s">
         <v>67</v>
       </c>
@@ -1964,14 +1980,14 @@
         <v>67</v>
       </c>
       <c r="AP3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AQ3" s="2" t="s">
+      <c r="AR3" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="AR3" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AS3" s="2" t="s">
         <v>67</v>
       </c>
@@ -1979,31 +1995,31 @@
         <v>67</v>
       </c>
       <c r="AU3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AV3" s="2" t="s">
+      <c r="AW3" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="AW3" s="2" t="s">
+      <c r="AX3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AX3" s="2" t="s">
+      <c r="AY3" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="AY3" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AZ3" s="2" t="s">
         <v>67</v>
       </c>
       <c r="BA3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="BB3" s="2" t="s">
+      <c r="BC3" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="BC3" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="BD3" s="2" t="s">
         <v>105</v>
@@ -2015,7 +2031,7 @@
         <v>105</v>
       </c>
       <c r="BG3" s="2" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="BH3" s="2" t="s">
         <v>67</v>
@@ -2027,22 +2043,26 @@
         <v>67</v>
       </c>
       <c r="BK3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BL3" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BM3" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN3" s="2" t="s">
         <v>84</v>
       </c>
       <c r="BO3" s="2" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ3" s="2"/>
     </row>
-    <row r="4" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:69" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>134</v>
       </c>
@@ -2074,14 +2094,14 @@
         <v>66</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="N4" s="2" t="s">
         <v>67</v>
       </c>
@@ -2101,62 +2121,62 @@
         <v>67</v>
       </c>
       <c r="T4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U4" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="X4" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="Y4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z4" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="AA4" s="2" t="s">
         <v>295</v>
       </c>
       <c r="AB4" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC4" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AC4" s="2" t="s">
+      <c r="AD4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="AD4" s="2" t="s">
+      <c r="AE4" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="AE4" s="2" t="s">
+      <c r="AF4" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="AF4" s="2" t="s">
+      <c r="AG4" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="AG4" s="2" t="s">
+      <c r="AH4" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="AH4" s="2" t="s">
+      <c r="AI4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AI4" s="2" t="s">
+      <c r="AJ4" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AJ4" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AK4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL4" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="AL4" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AM4" s="2" t="s">
         <v>67</v>
       </c>
@@ -2167,11 +2187,11 @@
         <v>67</v>
       </c>
       <c r="AP4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ4" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="AQ4" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AR4" s="2" t="s">
         <v>67</v>
       </c>
@@ -2179,35 +2199,35 @@
         <v>67</v>
       </c>
       <c r="AT4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AU4" s="2" t="s">
+      <c r="AV4" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AV4" s="2" t="s">
+      <c r="AW4" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="AW4" s="2" t="s">
+      <c r="AX4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AX4" s="2" t="s">
+      <c r="AY4" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="AY4" s="2" t="s">
+      <c r="AZ4" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="AZ4" s="2" t="s">
+      <c r="BA4" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="BA4" s="2" t="s">
+      <c r="BB4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="BB4" s="2" t="s">
+      <c r="BC4" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="BC4" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BD4" s="2" t="s">
         <v>67</v>
       </c>
@@ -2230,22 +2250,26 @@
         <v>67</v>
       </c>
       <c r="BK4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BL4" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BM4" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN4" s="2" t="s">
         <v>84</v>
       </c>
       <c r="BO4" s="2" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ4" s="2"/>
     </row>
-    <row r="5" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:69" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>180</v>
       </c>
@@ -2277,20 +2301,20 @@
         <v>66</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="P5" s="2" t="s">
         <v>67</v>
       </c>
@@ -2304,62 +2328,62 @@
         <v>67</v>
       </c>
       <c r="T5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U5" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="V5" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="W5" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="X5" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="Y5" s="2" t="s">
         <v>67</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>295</v>
+        <v>67</v>
       </c>
       <c r="AA5" s="2" t="s">
         <v>295</v>
       </c>
       <c r="AB5" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC5" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AC5" s="2" t="s">
+      <c r="AD5" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="AD5" s="2" t="s">
+      <c r="AE5" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="AE5" s="2" t="s">
+      <c r="AF5" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AF5" s="2" t="s">
+      <c r="AG5" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="AG5" s="2" t="s">
+      <c r="AH5" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="AH5" s="2" t="s">
+      <c r="AI5" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="AI5" s="2" t="s">
+      <c r="AJ5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AJ5" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AK5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL5" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="AL5" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AM5" s="2" t="s">
         <v>67</v>
       </c>
@@ -2370,47 +2394,47 @@
         <v>67</v>
       </c>
       <c r="AP5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ5" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AQ5" s="2" t="s">
+      <c r="AR5" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="AR5" s="2" t="s">
+      <c r="AS5" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AS5" s="2" t="s">
+      <c r="AT5" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="AT5" s="2" t="s">
+      <c r="AU5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AU5" s="2" t="s">
+      <c r="AV5" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AV5" s="2" t="s">
+      <c r="AW5" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="AW5" s="2" t="s">
+      <c r="AX5" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="AX5" s="2" t="s">
+      <c r="AY5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AY5" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AZ5" s="2" t="s">
         <v>67</v>
       </c>
       <c r="BA5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB5" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="BB5" s="2" t="s">
+      <c r="BC5" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="BC5" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BD5" s="2" t="s">
         <v>67</v>
       </c>
@@ -2433,22 +2457,26 @@
         <v>67</v>
       </c>
       <c r="BK5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BL5" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BM5" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN5" s="2" t="s">
         <v>84</v>
       </c>
       <c r="BO5" s="2" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ5" s="2"/>
     </row>
-    <row r="6" spans="1:67" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:69" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>193</v>
       </c>
@@ -2480,20 +2508,20 @@
         <v>66</v>
       </c>
       <c r="K6" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="M6" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="M6" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="N6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="O6" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="P6" s="8" t="s">
         <v>67</v>
       </c>
@@ -2507,62 +2535,62 @@
         <v>67</v>
       </c>
       <c r="T6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="U6" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="U6" s="8" t="s">
+      <c r="V6" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="V6" s="8" t="s">
+      <c r="W6" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="W6" s="8" t="s">
+      <c r="X6" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="X6" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="Y6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z6" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="Z6" s="8" t="s">
-        <v>295</v>
       </c>
       <c r="AA6" s="8" t="s">
         <v>295</v>
       </c>
       <c r="AB6" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC6" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="AC6" s="8" t="s">
+      <c r="AD6" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="AD6" s="8" t="s">
+      <c r="AE6" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="AE6" s="8" t="s">
+      <c r="AF6" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="AF6" s="8" t="s">
+      <c r="AG6" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="AG6" s="8" t="s">
+      <c r="AH6" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="AH6" s="8" t="s">
+      <c r="AI6" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="AI6" s="8" t="s">
+      <c r="AJ6" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="AJ6" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="AK6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL6" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="AL6" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="AM6" s="8" t="s">
         <v>67</v>
       </c>
@@ -2573,14 +2601,14 @@
         <v>67</v>
       </c>
       <c r="AP6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ6" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="AQ6" s="8" t="s">
+      <c r="AR6" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="AR6" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="AS6" s="8" t="s">
         <v>67</v>
       </c>
@@ -2588,44 +2616,44 @@
         <v>67</v>
       </c>
       <c r="AU6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV6" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AV6" s="8" t="s">
+      <c r="AW6" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="AW6" s="8" t="s">
+      <c r="AX6" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="AX6" s="8" t="s">
+      <c r="AY6" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="AY6" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="AZ6" s="8" t="s">
         <v>67</v>
       </c>
       <c r="BA6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB6" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="BB6" s="8" t="s">
+      <c r="BC6" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="BC6" s="8" t="s">
+      <c r="BD6" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="BD6" s="8" t="s">
+      <c r="BE6" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="BE6" s="8" t="s">
+      <c r="BF6" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="BF6" s="8" t="s">
+      <c r="BG6" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="BG6" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="BH6" s="8" t="s">
         <v>67</v>
       </c>
@@ -2636,22 +2664,26 @@
         <v>67</v>
       </c>
       <c r="BK6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL6" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="BL6" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="BM6" s="8" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN6" s="8" t="s">
         <v>84</v>
       </c>
       <c r="BO6" s="8" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ6" s="8"/>
     </row>
-    <row r="7" spans="1:67" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:69" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>193</v>
       </c>
@@ -2683,20 +2715,20 @@
         <v>66</v>
       </c>
       <c r="K7" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="M7" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="M7" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="N7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="O7" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="P7" s="8" t="s">
         <v>67</v>
       </c>
@@ -2710,62 +2742,62 @@
         <v>67</v>
       </c>
       <c r="T7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="U7" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="U7" s="8" t="s">
+      <c r="V7" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="V7" s="8" t="s">
+      <c r="W7" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="W7" s="8" t="s">
+      <c r="X7" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="X7" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="Y7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z7" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="Z7" s="8" t="s">
-        <v>295</v>
       </c>
       <c r="AA7" s="8" t="s">
         <v>295</v>
       </c>
       <c r="AB7" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC7" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="AC7" s="8" t="s">
+      <c r="AD7" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="AD7" s="8" t="s">
+      <c r="AE7" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="AE7" s="8" t="s">
+      <c r="AF7" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="AF7" s="8" t="s">
+      <c r="AG7" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="AG7" s="8" t="s">
+      <c r="AH7" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="AH7" s="8" t="s">
+      <c r="AI7" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="AI7" s="8" t="s">
+      <c r="AJ7" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="AJ7" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="AK7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL7" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="AL7" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="AM7" s="8" t="s">
         <v>67</v>
       </c>
@@ -2776,14 +2808,14 @@
         <v>67</v>
       </c>
       <c r="AP7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ7" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="AQ7" s="8" t="s">
+      <c r="AR7" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="AR7" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="AS7" s="8" t="s">
         <v>67</v>
       </c>
@@ -2791,44 +2823,44 @@
         <v>67</v>
       </c>
       <c r="AU7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV7" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AV7" s="8" t="s">
+      <c r="AW7" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="AW7" s="8" t="s">
+      <c r="AX7" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="AX7" s="8" t="s">
+      <c r="AY7" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AY7" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="AZ7" s="8" t="s">
         <v>67</v>
       </c>
       <c r="BA7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB7" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="BB7" s="8" t="s">
+      <c r="BC7" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="BC7" s="8" t="s">
+      <c r="BD7" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="BD7" s="8" t="s">
+      <c r="BE7" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="BE7" s="8" t="s">
+      <c r="BF7" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="BF7" s="8" t="s">
+      <c r="BG7" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="BG7" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="BH7" s="8" t="s">
         <v>67</v>
       </c>
@@ -2839,22 +2871,26 @@
         <v>67</v>
       </c>
       <c r="BK7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL7" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="BL7" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="BM7" s="8" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN7" s="8" t="s">
         <v>84</v>
       </c>
       <c r="BO7" s="8" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ7" s="8"/>
     </row>
-    <row r="8" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:69" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>202</v>
       </c>
@@ -2886,20 +2922,20 @@
         <v>66</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>204</v>
       </c>
       <c r="N8" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="O8" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="P8" s="2" t="s">
         <v>67</v>
       </c>
@@ -2913,62 +2949,62 @@
         <v>67</v>
       </c>
       <c r="T8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U8" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="V8" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="V8" s="2" t="s">
+      <c r="W8" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="X8" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="Y8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z8" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="Z8" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="AA8" s="2" t="s">
         <v>295</v>
       </c>
       <c r="AB8" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AC8" s="2" t="s">
+      <c r="AD8" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="AD8" s="2" t="s">
+      <c r="AE8" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="AE8" s="2" t="s">
+      <c r="AF8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AF8" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AG8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH8" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="AH8" s="2" t="s">
+      <c r="AI8" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="AI8" s="2" t="s">
+      <c r="AJ8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AJ8" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AK8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL8" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="AL8" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AM8" s="2" t="s">
         <v>67</v>
       </c>
@@ -2979,47 +3015,47 @@
         <v>67</v>
       </c>
       <c r="AP8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ8" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AQ8" s="2" t="s">
+      <c r="AR8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AR8" s="2" t="s">
+      <c r="AS8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AS8" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AT8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AU8" s="2" t="s">
+      <c r="AV8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AV8" s="2" t="s">
+      <c r="AW8" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="AW8" s="2" t="s">
+      <c r="AX8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AX8" s="2" t="s">
+      <c r="AY8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AY8" s="2" t="s">
+      <c r="AZ8" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AZ8" s="2" t="s">
+      <c r="BA8" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="BA8" s="2" t="s">
+      <c r="BB8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="BB8" s="2" t="s">
+      <c r="BC8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="BC8" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BD8" s="2" t="s">
         <v>67</v>
       </c>
@@ -3042,22 +3078,26 @@
         <v>67</v>
       </c>
       <c r="BK8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BL8" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BM8" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN8" s="2" t="s">
         <v>84</v>
       </c>
       <c r="BO8" s="2" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ8" s="2"/>
     </row>
-    <row r="9" spans="1:67" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:69" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>211</v>
       </c>
@@ -3089,20 +3129,20 @@
         <v>66</v>
       </c>
       <c r="K9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="M9" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="N9" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="O9" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="O9" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="P9" s="4" t="s">
         <v>67</v>
       </c>
@@ -3115,63 +3155,63 @@
       <c r="S9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="T9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="U9" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="U9" s="4" t="s">
+      <c r="V9" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="V9" s="2" t="s">
+      <c r="W9" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="W9" s="2" t="s">
+      <c r="X9" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="X9" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="Y9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z9" s="4" t="s">
         <v>217</v>
-      </c>
-      <c r="Z9" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="AA9" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="AB9" s="4" t="s">
+      <c r="AB9" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC9" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AC9" s="4" t="s">
+      <c r="AD9" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="AD9" s="4" t="s">
+      <c r="AE9" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="AE9" s="4" t="s">
+      <c r="AF9" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="AF9" s="4" t="s">
+      <c r="AG9" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="AG9" s="4" t="s">
+      <c r="AH9" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="AH9" s="4" t="s">
+      <c r="AI9" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="AI9" s="4" t="s">
+      <c r="AJ9" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="AJ9" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="AK9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL9" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="AL9" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="AM9" s="4" t="s">
         <v>67</v>
       </c>
@@ -3182,47 +3222,47 @@
         <v>67</v>
       </c>
       <c r="AP9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ9" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="AQ9" s="4" t="s">
+      <c r="AR9" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="AR9" s="4" t="s">
+      <c r="AS9" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="AS9" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="AT9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU9" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AU9" s="4" t="s">
+      <c r="AV9" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AV9" s="4" t="s">
+      <c r="AW9" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="AW9" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="AX9" s="4" t="s">
         <v>78</v>
       </c>
       <c r="AY9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ9" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="AZ9" s="4" t="s">
+      <c r="BA9" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="BA9" s="4" t="s">
+      <c r="BB9" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BB9" s="4" t="s">
+      <c r="BC9" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="BC9" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="BD9" s="4" t="s">
         <v>67</v>
       </c>
@@ -3245,22 +3285,26 @@
         <v>67</v>
       </c>
       <c r="BK9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BL9" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="BM9" s="4" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN9" s="4" t="s">
         <v>84</v>
       </c>
       <c r="BO9" s="4" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ9" s="4"/>
     </row>
-    <row r="10" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:69" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>227</v>
       </c>
@@ -3292,20 +3336,20 @@
         <v>66</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="P10" s="2" t="s">
         <v>67</v>
       </c>
@@ -3319,62 +3363,62 @@
         <v>67</v>
       </c>
       <c r="T10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U10" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="U10" s="2" t="s">
+      <c r="V10" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="V10" s="2" t="s">
+      <c r="W10" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="W10" s="2" t="s">
+      <c r="X10" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="X10" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="Y10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z10" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="Z10" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="AA10" s="2" t="s">
         <v>295</v>
       </c>
       <c r="AB10" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC10" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AC10" s="2" t="s">
+      <c r="AD10" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="AD10" s="2" t="s">
+      <c r="AE10" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AE10" s="2" t="s">
+      <c r="AF10" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="AF10" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AG10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH10" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="AH10" s="2" t="s">
+      <c r="AI10" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="AI10" s="2" t="s">
+      <c r="AJ10" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AJ10" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AK10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL10" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="AL10" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AM10" s="2" t="s">
         <v>67</v>
       </c>
@@ -3385,47 +3429,47 @@
         <v>67</v>
       </c>
       <c r="AP10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ10" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AQ10" s="2" t="s">
+      <c r="AR10" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AR10" s="2" t="s">
+      <c r="AS10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AS10" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AT10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AU10" s="2" t="s">
+      <c r="AV10" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AV10" s="2" t="s">
+      <c r="AW10" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="AW10" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="AX10" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AY10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ10" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="AZ10" s="2" t="s">
+      <c r="BA10" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="BA10" s="2" t="s">
+      <c r="BB10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="BB10" s="2" t="s">
+      <c r="BC10" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="BC10" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BD10" s="2" t="s">
         <v>67</v>
       </c>
@@ -3448,22 +3492,26 @@
         <v>67</v>
       </c>
       <c r="BK10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL10" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BL10" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BM10" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN10" s="2" t="s">
         <v>84</v>
       </c>
       <c r="BO10" s="2" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ10" s="2"/>
     </row>
-    <row r="11" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:69" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>238</v>
       </c>
@@ -3495,20 +3543,20 @@
         <v>66</v>
       </c>
       <c r="K11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="M11" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="N11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O11" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="O11" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="P11" s="2" t="s">
         <v>67</v>
       </c>
@@ -3522,62 +3570,62 @@
         <v>67</v>
       </c>
       <c r="T11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U11" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="U11" s="2" t="s">
+      <c r="V11" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="V11" s="2" t="s">
+      <c r="W11" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="W11" s="2" t="s">
+      <c r="X11" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="X11" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="Y11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z11" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="Z11" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="AA11" s="2" t="s">
         <v>295</v>
       </c>
       <c r="AB11" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AC11" s="2" t="s">
+      <c r="AD11" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="AD11" s="2" t="s">
+      <c r="AE11" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="AE11" s="2" t="s">
+      <c r="AF11" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="AF11" s="2" t="s">
+      <c r="AG11" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="AG11" s="2" t="s">
+      <c r="AH11" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="AH11" s="2" t="s">
+      <c r="AI11" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="AI11" s="2" t="s">
+      <c r="AJ11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AJ11" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AK11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL11" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="AL11" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AM11" s="2" t="s">
         <v>67</v>
       </c>
@@ -3588,14 +3636,14 @@
         <v>67</v>
       </c>
       <c r="AP11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ11" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AQ11" s="2" t="s">
+      <c r="AR11" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="AR11" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AS11" s="2" t="s">
         <v>67</v>
       </c>
@@ -3603,31 +3651,31 @@
         <v>67</v>
       </c>
       <c r="AU11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV11" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AV11" s="2" t="s">
+      <c r="AW11" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="AW11" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="AX11" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AY11" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="AZ11" s="2" t="s">
         <v>67</v>
       </c>
       <c r="BA11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="BB11" s="2" t="s">
+      <c r="BC11" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="BC11" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="BD11" s="2" t="s">
         <v>105</v>
@@ -3639,7 +3687,7 @@
         <v>105</v>
       </c>
       <c r="BG11" s="2" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="BH11" s="2" t="s">
         <v>67</v>
@@ -3651,22 +3699,26 @@
         <v>67</v>
       </c>
       <c r="BK11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL11" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BL11" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BM11" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN11" s="2" t="s">
         <v>84</v>
       </c>
       <c r="BO11" s="2" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ11" s="2"/>
     </row>
-    <row r="12" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:69" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>248</v>
       </c>
@@ -3698,20 +3750,20 @@
         <v>66</v>
       </c>
       <c r="K12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="M12" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="N12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O12" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="O12" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="P12" s="2" t="s">
         <v>67</v>
       </c>
@@ -3725,62 +3777,62 @@
         <v>67</v>
       </c>
       <c r="T12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U12" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="U12" s="2" t="s">
+      <c r="V12" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="V12" s="2" t="s">
+      <c r="W12" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="W12" s="2" t="s">
+      <c r="X12" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="X12" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="Y12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z12" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="Z12" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="AA12" s="2" t="s">
         <v>295</v>
       </c>
       <c r="AB12" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC12" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AC12" s="2" t="s">
+      <c r="AD12" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="AD12" s="2" t="s">
+      <c r="AE12" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="AE12" s="2" t="s">
+      <c r="AF12" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="AF12" s="2" t="s">
+      <c r="AG12" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="AG12" s="2" t="s">
+      <c r="AH12" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="AH12" s="2" t="s">
+      <c r="AI12" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="AI12" s="2" t="s">
+      <c r="AJ12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AJ12" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AK12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL12" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="AL12" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AM12" s="2" t="s">
         <v>67</v>
       </c>
@@ -3791,14 +3843,14 @@
         <v>67</v>
       </c>
       <c r="AP12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ12" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AQ12" s="2" t="s">
+      <c r="AR12" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="AR12" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AS12" s="2" t="s">
         <v>67</v>
       </c>
@@ -3806,31 +3858,31 @@
         <v>67</v>
       </c>
       <c r="AU12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV12" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AV12" s="2" t="s">
+      <c r="AW12" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="AW12" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="AX12" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AY12" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="AZ12" s="2" t="s">
         <v>67</v>
       </c>
       <c r="BA12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="BB12" s="2" t="s">
+      <c r="BC12" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="BC12" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="BD12" s="2" t="s">
         <v>105</v>
@@ -3839,11 +3891,11 @@
         <v>105</v>
       </c>
       <c r="BF12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="BG12" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="BG12" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BH12" s="2" t="s">
         <v>67</v>
       </c>
@@ -3854,22 +3906,26 @@
         <v>67</v>
       </c>
       <c r="BK12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BL12" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BM12" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN12" s="2" t="s">
         <v>84</v>
       </c>
       <c r="BO12" s="2" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ12" s="2"/>
     </row>
-    <row r="13" spans="1:67" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:69" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>257</v>
       </c>
@@ -3901,20 +3957,20 @@
         <v>66</v>
       </c>
       <c r="K13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="M13" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="O13" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="O13" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="P13" s="4" t="s">
         <v>67</v>
       </c>
@@ -3927,63 +3983,63 @@
       <c r="S13" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="T13" s="2" t="s">
+      <c r="T13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="U13" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="U13" s="2" t="s">
+      <c r="V13" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="V13" s="2" t="s">
+      <c r="W13" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="W13" s="2" t="s">
+      <c r="X13" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="X13" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="Y13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z13" s="4" t="s">
         <v>262</v>
-      </c>
-      <c r="Z13" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="AA13" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="AB13" s="4" t="s">
+      <c r="AB13" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC13" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AC13" s="4" t="s">
+      <c r="AD13" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="AD13" s="4" t="s">
+      <c r="AE13" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="AE13" s="4" t="s">
+      <c r="AF13" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="AF13" s="4" t="s">
+      <c r="AG13" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="AG13" s="4" t="s">
+      <c r="AH13" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="AH13" s="4" t="s">
+      <c r="AI13" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="AI13" s="4" t="s">
+      <c r="AJ13" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="AJ13" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="AK13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL13" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="AL13" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="AM13" s="4" t="s">
         <v>67</v>
       </c>
@@ -3994,47 +4050,47 @@
         <v>67</v>
       </c>
       <c r="AP13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ13" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="AQ13" s="4" t="s">
+      <c r="AR13" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="AR13" s="4" t="s">
+      <c r="AS13" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="AS13" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="AT13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU13" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AU13" s="4" t="s">
+      <c r="AV13" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AV13" s="4" t="s">
+      <c r="AW13" s="4" t="s">
         <v>268</v>
-      </c>
-      <c r="AW13" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="AX13" s="4" t="s">
         <v>78</v>
       </c>
       <c r="AY13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ13" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="AZ13" s="4" t="s">
+      <c r="BA13" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="BA13" s="4" t="s">
+      <c r="BB13" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BB13" s="4" t="s">
+      <c r="BC13" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="BC13" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="BD13" s="4" t="s">
         <v>67</v>
       </c>
@@ -4057,22 +4113,26 @@
         <v>67</v>
       </c>
       <c r="BK13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL13" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BL13" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="BM13" s="4" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN13" s="4" t="s">
         <v>84</v>
       </c>
       <c r="BO13" s="4" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ13" s="4"/>
     </row>
-    <row r="14" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:69" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>271</v>
       </c>
@@ -4104,20 +4164,20 @@
         <v>66</v>
       </c>
       <c r="K14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="M14" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="N14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O14" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="O14" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="P14" s="2" t="s">
         <v>67</v>
       </c>
@@ -4131,62 +4191,62 @@
         <v>67</v>
       </c>
       <c r="T14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U14" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="U14" s="2" t="s">
+      <c r="V14" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="V14" s="2" t="s">
+      <c r="W14" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="W14" s="2" t="s">
+      <c r="X14" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="X14" s="2" t="s">
+      <c r="Y14" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="Y14" s="2" t="s">
+      <c r="Z14" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="Z14" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="AA14" s="2" t="s">
         <v>295</v>
       </c>
       <c r="AB14" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AC14" s="2" t="s">
+      <c r="AD14" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="AD14" s="2" t="s">
+      <c r="AE14" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AE14" s="2" t="s">
+      <c r="AF14" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AF14" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AG14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH14" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="AH14" s="2" t="s">
+      <c r="AI14" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="AI14" s="2" t="s">
+      <c r="AJ14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AJ14" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AK14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL14" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="AL14" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AM14" s="2" t="s">
         <v>67</v>
       </c>
@@ -4197,47 +4257,47 @@
         <v>67</v>
       </c>
       <c r="AP14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AQ14" s="2" t="s">
+      <c r="AR14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AR14" s="2" t="s">
+      <c r="AS14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AS14" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AT14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AU14" s="2" t="s">
+      <c r="AV14" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AV14" s="2" t="s">
+      <c r="AW14" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="AW14" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="AX14" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AY14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ14" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="AZ14" s="2" t="s">
+      <c r="BA14" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="BA14" s="2" t="s">
+      <c r="BB14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="BB14" s="2" t="s">
+      <c r="BC14" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="BC14" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BD14" s="2" t="s">
         <v>67</v>
       </c>
@@ -4260,22 +4320,26 @@
         <v>67</v>
       </c>
       <c r="BK14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL14" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BL14" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BM14" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN14" s="2" t="s">
         <v>84</v>
       </c>
       <c r="BO14" s="2" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ14" s="2"/>
     </row>
-    <row r="15" spans="1:67" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:69" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>193</v>
       </c>
@@ -4307,20 +4371,20 @@
         <v>66</v>
       </c>
       <c r="K15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L15" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="M15" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="N15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="O15" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="O15" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="P15" s="6" t="s">
         <v>67</v>
       </c>
@@ -4334,62 +4398,62 @@
         <v>67</v>
       </c>
       <c r="T15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="U15" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="U15" s="6" t="s">
+      <c r="V15" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="V15" s="6" t="s">
+      <c r="W15" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="W15" s="6" t="s">
+      <c r="X15" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="X15" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="Y15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z15" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="Z15" s="6" t="s">
-        <v>295</v>
       </c>
       <c r="AA15" s="6" t="s">
         <v>295</v>
       </c>
       <c r="AB15" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC15" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="AC15" s="6" t="s">
+      <c r="AD15" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="AD15" s="6" t="s">
+      <c r="AE15" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="AE15" s="6" t="s">
+      <c r="AF15" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="AF15" s="6" t="s">
+      <c r="AG15" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="AG15" s="6" t="s">
+      <c r="AH15" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="AH15" s="6" t="s">
+      <c r="AI15" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="AI15" s="6" t="s">
+      <c r="AJ15" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="AJ15" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="AK15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL15" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="AL15" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="AM15" s="6" t="s">
         <v>67</v>
       </c>
@@ -4400,14 +4464,14 @@
         <v>67</v>
       </c>
       <c r="AP15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ15" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="AQ15" s="6" t="s">
+      <c r="AR15" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="AR15" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="AS15" s="6" t="s">
         <v>67</v>
       </c>
@@ -4415,44 +4479,44 @@
         <v>67</v>
       </c>
       <c r="AU15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV15" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AV15" s="6" t="s">
+      <c r="AW15" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="AW15" s="6" t="s">
+      <c r="AX15" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AX15" s="6" t="s">
+      <c r="AY15" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AY15" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="AZ15" s="6" t="s">
         <v>67</v>
       </c>
       <c r="BA15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB15" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="BB15" s="6" t="s">
+      <c r="BC15" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="BC15" s="6" t="s">
+      <c r="BD15" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="BD15" s="6" t="s">
+      <c r="BE15" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="BE15" s="6" t="s">
+      <c r="BF15" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="BF15" s="6" t="s">
+      <c r="BG15" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="BG15" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="BH15" s="6" t="s">
         <v>67</v>
       </c>
@@ -4463,22 +4527,26 @@
         <v>67</v>
       </c>
       <c r="BK15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL15" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="BL15" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="BM15" s="6" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN15" s="6" t="s">
         <v>84</v>
       </c>
       <c r="BO15" s="6" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ15" s="6"/>
     </row>
-    <row r="16" spans="1:67" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:69" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>193</v>
       </c>
@@ -4510,20 +4578,20 @@
         <v>66</v>
       </c>
       <c r="K16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L16" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="L16" s="6" t="s">
+      <c r="M16" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="M16" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="N16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="O16" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="O16" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="P16" s="6" t="s">
         <v>67</v>
       </c>
@@ -4537,62 +4605,62 @@
         <v>67</v>
       </c>
       <c r="T16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="U16" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="U16" s="6" t="s">
+      <c r="V16" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="V16" s="6" t="s">
+      <c r="W16" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="W16" s="6" t="s">
+      <c r="X16" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="X16" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="Y16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z16" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="Z16" s="6" t="s">
-        <v>295</v>
       </c>
       <c r="AA16" s="6" t="s">
         <v>295</v>
       </c>
       <c r="AB16" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC16" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="AC16" s="6" t="s">
+      <c r="AD16" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="AD16" s="6" t="s">
+      <c r="AE16" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="AE16" s="6" t="s">
+      <c r="AF16" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="AF16" s="6" t="s">
+      <c r="AG16" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="AG16" s="6" t="s">
+      <c r="AH16" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="AH16" s="6" t="s">
+      <c r="AI16" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="AI16" s="6" t="s">
+      <c r="AJ16" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="AJ16" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="AK16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL16" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="AL16" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="AM16" s="6" t="s">
         <v>67</v>
       </c>
@@ -4603,14 +4671,14 @@
         <v>67</v>
       </c>
       <c r="AP16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ16" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="AQ16" s="6" t="s">
+      <c r="AR16" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="AR16" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="AS16" s="6" t="s">
         <v>67</v>
       </c>
@@ -4618,44 +4686,44 @@
         <v>67</v>
       </c>
       <c r="AU16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV16" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AV16" s="6" t="s">
+      <c r="AW16" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="AW16" s="6" t="s">
+      <c r="AX16" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AX16" s="6" t="s">
+      <c r="AY16" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AY16" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="AZ16" s="6" t="s">
         <v>67</v>
       </c>
       <c r="BA16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB16" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="BB16" s="6" t="s">
+      <c r="BC16" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="BC16" s="6" t="s">
+      <c r="BD16" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="BD16" s="6" t="s">
+      <c r="BE16" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="BE16" s="6" t="s">
+      <c r="BF16" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="BF16" s="6" t="s">
+      <c r="BG16" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="BG16" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="BH16" s="6" t="s">
         <v>67</v>
       </c>
@@ -4666,22 +4734,26 @@
         <v>67</v>
       </c>
       <c r="BK16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL16" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="BL16" s="6" t="s">
-        <v>67</v>
-      </c>
       <c r="BM16" s="6" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN16" s="6" t="s">
         <v>84</v>
       </c>
       <c r="BO16" s="6" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ16" s="6"/>
     </row>
-    <row r="17" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:69" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>281</v>
       </c>
@@ -4713,20 +4785,20 @@
         <v>66</v>
       </c>
       <c r="K17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="N17" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="O17" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="P17" s="2" t="s">
         <v>67</v>
       </c>
@@ -4740,62 +4812,62 @@
         <v>67</v>
       </c>
       <c r="T17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="U17" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="U17" s="2" t="s">
+      <c r="V17" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="V17" s="2" t="s">
+      <c r="W17" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="W17" s="2" t="s">
+      <c r="X17" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="X17" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="Y17" s="2" t="s">
         <v>67</v>
       </c>
       <c r="Z17" s="2" t="s">
-        <v>295</v>
+        <v>67</v>
       </c>
       <c r="AA17" s="2" t="s">
         <v>295</v>
       </c>
       <c r="AB17" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AC17" s="2" t="s">
+      <c r="AD17" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="AD17" s="2" t="s">
+      <c r="AE17" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="AE17" s="2" t="s">
+      <c r="AF17" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="AF17" s="2" t="s">
+      <c r="AG17" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="AG17" s="2" t="s">
+      <c r="AH17" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="AH17" s="2" t="s">
+      <c r="AI17" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="AI17" s="2" t="s">
+      <c r="AJ17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AJ17" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AK17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL17" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="AL17" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AM17" s="2" t="s">
         <v>67</v>
       </c>
@@ -4806,47 +4878,47 @@
         <v>67</v>
       </c>
       <c r="AP17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AQ17" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AQ17" s="2" t="s">
+      <c r="AR17" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="AR17" s="2" t="s">
+      <c r="AS17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AS17" s="2" t="s">
+      <c r="AT17" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="AT17" s="2" t="s">
+      <c r="AU17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AU17" s="2" t="s">
+      <c r="AV17" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AV17" s="2" t="s">
+      <c r="AW17" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="AW17" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="AX17" s="2" t="s">
         <v>78</v>
       </c>
       <c r="AY17" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="AZ17" s="2" t="s">
         <v>67</v>
       </c>
       <c r="BA17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="BB17" s="2" t="s">
+      <c r="BC17" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="BC17" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BD17" s="2" t="s">
         <v>67</v>
       </c>
@@ -4869,20 +4941,24 @@
         <v>67</v>
       </c>
       <c r="BK17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BL17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="BL17" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="BM17" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="BN17" s="2" t="s">
         <v>84</v>
       </c>
       <c r="BO17" s="2" t="s">
-        <v>67</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="BP17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ17" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>